<commit_message>
fix : flat error
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -7,11 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="손상현황표" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="시설물 현황" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="손상현황표" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'손상현황표'!$A$2:$J$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'손상현황표'!$A$2:$J$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,7 +20,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -29,12 +32,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCCC"/>
+        <bgColor rgb="00CCCCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +58,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -419,6 +437,225 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>□ 시설물 현황</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>가. 일반현황</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>시설물명</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>정부춘천</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>시설물번호</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>AR2003-0009512</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>시설물위치</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>AR2003-0009512</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>준공일자</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>44559</v>
+      </c>
+      <c r="G5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>용도</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>공공업무</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>시설물규모</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>지하1층</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>구조형식</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>철근</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>부대시설</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr"/>
+      <c r="G7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>종별</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>3층</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>전차안전등급</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>b등급</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>점검결과안전등급</t>
+        </is>
+      </c>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>b등급(8.7점)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>규모 및 제원 추가사항</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>없음</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -431,13 +668,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J4"/>
+  <dimension ref="A2:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,156 +686,102 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>구분</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>층수</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>위치</t>
         </is>
       </c>
-      <c r="D2" s="1" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>부재</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>점검내용</t>
         </is>
       </c>
-      <c r="F2" s="1" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>개소</t>
         </is>
       </c>
-      <c r="G2" s="1" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>현황번호</t>
         </is>
       </c>
-      <c r="H2" s="1" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>진행유무</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="I2" s="4" t="inlineStr">
         <is>
           <t>발생원인</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="J2" s="4" t="inlineStr">
         <is>
           <t>비고</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>5층</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>옥탑층</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>물탱크실</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="D3" s="4" t="inlineStr">
         <is>
           <t>벽재</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>0.2* 4,500 수직</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>0.2x3500 수직, 수평</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="inlineStr">
         <is>
           <t>신규</t>
         </is>
       </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>건조수축</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>사진1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>5층</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>복도</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>슬래브</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>텍스누스흔적</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>신규</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>우수유입</t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t>사진5</t>
-        </is>
-      </c>
+      <c r="I3" s="4" t="inlineStr">
+        <is>
+          <t>모름</t>
+        </is>
+      </c>
+      <c r="J3" s="4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
crack model 수정, create, update 수정
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -155,7 +155,7 @@
       <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4762500" cy="2828925"/>
+    <ext cx="4762500" cy="1704975"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -180,7 +180,7 @@
       <row>42</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="4762500" cy="2781300"/>
+    <ext cx="4762500" cy="3609975"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -188,111 +188,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2047875" cy="1533525"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>2</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2047875" cy="1657350"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>4</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2047875" cy="1543050"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 3" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2047875" cy="1228725"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -656,7 +551,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>정부춘천지방함동청사</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D4" s="1" t="n"/>
@@ -667,7 +562,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>AR2003-0009511</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G4" s="1" t="n"/>
@@ -681,7 +576,7 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>AR2003-0009511</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" s="1" t="n"/>
@@ -691,7 +586,7 @@
         </is>
       </c>
       <c r="F5" s="3" t="n">
-        <v>37981</v>
+        <v>-693593</v>
       </c>
       <c r="G5" s="1" t="n"/>
     </row>
@@ -704,7 +599,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>공공업무시설</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D6" s="1" t="n"/>
@@ -715,7 +610,7 @@
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>지하1층, 지상5층</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G6" s="1" t="n"/>
@@ -729,7 +624,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>철근콘트리트구조</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" s="1" t="n"/>
@@ -740,7 +635,7 @@
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>11</t>
         </is>
       </c>
       <c r="G7" s="1" t="n"/>
@@ -754,7 +649,7 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>3층</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
@@ -764,7 +659,7 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>B등급</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
@@ -774,7 +669,7 @@
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>B등급(8.7점)</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -795,7 +690,7 @@
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C10" s="1" t="n"/>
@@ -1119,14 +1014,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B10:F13"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1139,78 +1034,8 @@
     <col width="27" customWidth="1" min="5" max="5"/>
     <col width="27" customWidth="1" min="6" max="6"/>
   </cols>
-  <sheetData>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>사진번호: 13</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>사진번호: 14</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>위치: 옥탑층이냐?물탱크실임 ㅋ</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>위치: 옥탑층이냐?물탱크실임 ㅋ</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>점검내용: 0.2* 4,500 수직</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>손상규모: None</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>점검내용: 0.2* 4,500 수직</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>손상규모: None</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>발생원인: 건조수축</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>진행유무: 신규</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>발생원인: 건조수축</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>진행유무: 신규</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1220,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J3"/>
+  <dimension ref="A2:I2"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1278,56 +1103,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>옥탑층이냐?</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>물탱크실임 ㅋ</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t>벽재</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>0.2* 4,500 수직</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H3" s="4" t="inlineStr">
-        <is>
-          <t>신규</t>
-        </is>
-      </c>
-      <c r="I3" s="4" t="inlineStr">
-        <is>
-          <t>건조수축</t>
-        </is>
-      </c>
-      <c r="J3" s="4" t="inlineStr">
-        <is>
-          <t>사진1</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>